<commit_message>
修改 key 属性排序至 formatProperties
</commit_message>
<xml_diff>
--- a/example/batchConvert/$tables.xlsx
+++ b/example/batchConvert/$tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luyi/splan-git/xlsx-fbs/example/batchConvert/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E4712E3-6E6A-BA42-BFE9-49C9A2922F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD64BFA-00C7-C24C-82FB-372DD77A511B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2300" windowWidth="38400" windowHeight="12120" xr2:uid="{89FDA258-6872-FE40-AC0D-7BDF8BC8DEC7}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -140,6 +140,10 @@
   </si>
   <si>
     <t>lowerProb</t>
+  </si>
+  <si>
+    <t>domain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -526,7 +530,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22580904-9B8E-6746-AACC-FD6B519A2E15}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
@@ -605,6 +609,14 @@
       </c>
       <c r="E5" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>